<commit_message>
wrong report submitted: uploading correct file
</commit_message>
<xml_diff>
--- a/Papers:Report/PSA final Projecct.xlsx
+++ b/Papers:Report/PSA final Projecct.xlsx
@@ -116,7 +116,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Sheet1!$A$3</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -131,12 +131,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$11</c:f>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -147,7 +147,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$A$4</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -162,12 +162,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$11</c:f>
+              <c:f>Sheet1!$B$4:$F$4</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -178,7 +178,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$A$5</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -193,12 +193,12 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$11</c:f>
+              <c:f>Sheet1!$B$5:$F$5</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -209,7 +209,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Sheet1!$A$6</c:f>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -224,53 +224,22 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$11</c:f>
+              <c:f>Sheet1!$B$6:$F$6</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="FF6D01"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$3:$F$11</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:axId val="1015486522"/>
-        <c:axId val="44903744"/>
+        <c:axId val="1704395495"/>
+        <c:axId val="1736681447"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1015486522"/>
+        <c:axId val="1704395495"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,10 +291,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44903744"/>
+        <c:crossAx val="1736681447"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44903744"/>
+        <c:axId val="1736681447"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,7 +369,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1015486522"/>
+        <c:crossAx val="1704395495"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -427,6 +396,324 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>N = 250000, N= 500000, N = 1000000, N = 2M and N = 4M</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FBBC04"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$F$5</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="34A853"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$F$6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="1893357297"/>
+        <c:axId val="1418966651"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1893357297"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Sorting using Array of Strings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1418966651"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1418966651"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1893357297"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -553,11 +840,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2068719597"/>
-        <c:axId val="1283355765"/>
+        <c:axId val="204329812"/>
+        <c:axId val="1092126687"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2068719597"/>
+        <c:axId val="204329812"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,10 +896,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1283355765"/>
+        <c:crossAx val="1092126687"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1283355765"/>
+        <c:axId val="1092126687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,294 +974,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2068719597"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="757575"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>LSD Radix Sort (Array String), MSD Radix Sort (Array String) and Dual Pivot QuickSort (Array String)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="4285F4"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="EA4335"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$F$4</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="FBBC04"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$5:$F$5</c:f>
-              <c:numCache/>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="414996547"/>
-        <c:axId val="1956413237"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="414996547"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>Sorting Name</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:spPr/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1956413237"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1956413237"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="CCCCCC">
-                  <a:alpha val="0"/>
-                </a:srgbClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t/>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr b="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="414996547"/>
+        <c:crossAx val="204329812"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1030,9 +1030,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -1056,8 +1056,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>

</xml_diff>